<commit_message>
(ABM-1181) - Initial Development Commit
</commit_message>
<xml_diff>
--- a/resources/fed_rtp_20/templates/Scenario SDF Performance Measures_template.xlsx
+++ b/resources/fed_rtp_20/templates/Scenario SDF Performance Measures_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gsc\OneDrive - San Diego Association of Governments\gsc\abm_2_reporting\resources\fed_rtp_20\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\TEMP\gks\abm_2_reporting\resources\fed_rtp_20\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{40DCBA3F-9C21-482E-BBF9-A15DE9B4AB93}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{80BBD119-11A0-4D3D-B1EE-DBD2833BC2E2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C6FC23-3D79-4F00-813F-E0DB00176B70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23265" windowHeight="9180" tabRatio="969" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23265" windowHeight="9180" tabRatio="969" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -1696,7 +1696,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -2198,6 +2198,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0"/>
@@ -2210,7 +2223,7 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="3" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="310">
+  <cellXfs count="315">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2750,20 +2763,6 @@
     <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="34" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="22" borderId="34" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2776,6 +2775,26 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="19" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2789,6 +2808,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="10" fillId="21" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="60% - Accent3" xfId="2" builtinId="40"/>
@@ -3168,16 +3192,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K265"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C243" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C252" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomRight" activeCell="G265" sqref="G265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="242" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="242" customWidth="1"/>
     <col min="2" max="2" width="51" style="242" customWidth="1"/>
     <col min="3" max="3" width="3.85546875" style="90" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" style="90" customWidth="1"/>
@@ -3956,10 +3980,10 @@
       <c r="J53" s="255"/>
     </row>
     <row r="54" spans="1:10" s="242" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="297" t="s">
+      <c r="A54" s="299" t="s">
         <v>332</v>
       </c>
-      <c r="B54" s="300" t="s">
+      <c r="B54" s="294" t="s">
         <v>333</v>
       </c>
       <c r="C54" s="254"/>
@@ -3972,10 +3996,10 @@
       <c r="J54" s="255"/>
     </row>
     <row r="55" spans="1:10" s="242" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="297" t="s">
+      <c r="A55" s="299" t="s">
         <v>335</v>
       </c>
-      <c r="B55" s="300" t="s">
+      <c r="B55" s="294" t="s">
         <v>336</v>
       </c>
       <c r="C55" s="254"/>
@@ -6926,20 +6950,20 @@
       <c r="J251" s="274"/>
     </row>
     <row r="252" spans="1:10" s="242" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A252" s="291" t="s">
+      <c r="A252" s="98" t="s">
         <v>327</v>
       </c>
-      <c r="B252" s="292" t="s">
+      <c r="B252" s="298" t="s">
         <v>328</v>
       </c>
       <c r="C252" s="256"/>
-      <c r="D252" s="301"/>
-      <c r="E252" s="301"/>
-      <c r="F252" s="301"/>
-      <c r="G252" s="301"/>
-      <c r="H252" s="301"/>
-      <c r="I252" s="301"/>
-      <c r="J252" s="301"/>
+      <c r="D252" s="295"/>
+      <c r="E252" s="295"/>
+      <c r="F252" s="295"/>
+      <c r="G252" s="295"/>
+      <c r="H252" s="295"/>
+      <c r="I252" s="295"/>
+      <c r="J252" s="295"/>
     </row>
     <row r="253" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="23" t="s">
@@ -6996,7 +7020,7 @@
       <c r="I256" s="270"/>
       <c r="J256" s="270"/>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B257" s="87" t="s">
         <v>44</v>
       </c>
@@ -7009,7 +7033,7 @@
       <c r="I257" s="270"/>
       <c r="J257" s="270"/>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B258" s="87" t="s">
         <v>45</v>
       </c>
@@ -7022,7 +7046,7 @@
       <c r="I258" s="270"/>
       <c r="J258" s="270"/>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A259" s="58"/>
       <c r="B259" s="87" t="s">
         <v>46</v>
@@ -7036,47 +7060,89 @@
       <c r="I259" s="270"/>
       <c r="J259" s="270"/>
     </row>
-    <row r="260" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A260" s="293" t="s">
+    <row r="260" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A260" s="297" t="s">
         <v>329</v>
       </c>
-      <c r="B260" s="293" t="s">
+      <c r="B260" s="297" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A261" s="294"/>
-      <c r="B261" s="294" t="s">
+      <c r="D260" s="275"/>
+      <c r="F260" s="313"/>
+      <c r="G260" s="313"/>
+      <c r="H260" s="313"/>
+      <c r="I260" s="313"/>
+      <c r="J260" s="313"/>
+      <c r="K260" s="314"/>
+    </row>
+    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B261" s="87" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A262" s="294"/>
-      <c r="B262" s="294" t="s">
+      <c r="C261" s="270"/>
+      <c r="D261" s="275"/>
+      <c r="E261" s="270"/>
+      <c r="F261" s="270"/>
+      <c r="G261" s="270"/>
+      <c r="H261" s="270"/>
+      <c r="I261" s="270"/>
+      <c r="J261" s="270"/>
+    </row>
+    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B262" s="87" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A263" s="294"/>
-      <c r="B263" s="294" t="s">
+      <c r="C262" s="270"/>
+      <c r="D262" s="275"/>
+      <c r="E262" s="270"/>
+      <c r="F262" s="270"/>
+      <c r="G262" s="270"/>
+      <c r="H262" s="270"/>
+      <c r="I262" s="270"/>
+      <c r="J262" s="270"/>
+    </row>
+    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B263" s="87" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A264" s="294"/>
-      <c r="B264" s="294" t="s">
+      <c r="C263" s="270"/>
+      <c r="D263" s="275"/>
+      <c r="E263" s="270"/>
+      <c r="F263" s="270"/>
+      <c r="G263" s="270"/>
+      <c r="H263" s="270"/>
+      <c r="I263" s="270"/>
+      <c r="J263" s="270"/>
+    </row>
+    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B264" s="87" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A265" s="294"/>
-      <c r="B265" s="294" t="s">
+      <c r="C264" s="270"/>
+      <c r="D264" s="275"/>
+      <c r="E264" s="270"/>
+      <c r="F264" s="270"/>
+      <c r="G264" s="270"/>
+      <c r="H264" s="270"/>
+      <c r="I264" s="270"/>
+      <c r="J264" s="270"/>
+    </row>
+    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B265" s="87" t="s">
         <v>29</v>
       </c>
+      <c r="C265" s="270"/>
+      <c r="D265" s="275"/>
+      <c r="E265" s="270"/>
+      <c r="F265" s="270"/>
+      <c r="G265" s="270"/>
+      <c r="H265" s="270"/>
+      <c r="I265" s="270"/>
+      <c r="J265" s="270"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="17" scale="81" fitToHeight="0" orientation="portrait"/>
+  <pageSetup paperSize="17" scale="81" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8040,11 +8106,11 @@
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
-      <c r="F3" s="307"/>
-      <c r="G3" s="308"/>
-      <c r="H3" s="308"/>
-      <c r="I3" s="308"/>
-      <c r="J3" s="309"/>
+      <c r="F3" s="309"/>
+      <c r="G3" s="310"/>
+      <c r="H3" s="310"/>
+      <c r="I3" s="310"/>
+      <c r="J3" s="311"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="87" t="s">
@@ -8283,8 +8349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8326,7 +8392,7 @@
       <c r="C2" s="107" t="s">
         <v>128</v>
       </c>
-      <c r="D2"/>
+      <c r="D2" s="237"/>
     </row>
     <row r="3" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="108" t="s">
@@ -8717,7 +8783,7 @@
       <c r="C31" s="116" t="s">
         <v>150</v>
       </c>
-      <c r="D31"/>
+      <c r="D31" s="237"/>
     </row>
     <row r="32" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="118" t="s">
@@ -8950,8 +9016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8959,7 +9025,7 @@
     <col min="1" max="1" width="9.140625" style="240" customWidth="1"/>
     <col min="2" max="2" width="40.5703125" style="138" customWidth="1"/>
     <col min="3" max="3" width="40.5703125" style="240" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="240" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="239" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="240" customWidth="1"/>
     <col min="6" max="9" width="15.5703125" style="240" customWidth="1"/>
     <col min="10" max="10" width="11.5703125" style="240" customWidth="1"/>
@@ -8977,7 +9043,7 @@
       <c r="C1" s="197" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="197"/>
+      <c r="D1" s="312"/>
       <c r="E1" s="197"/>
       <c r="F1" s="197"/>
       <c r="G1" s="197"/>
@@ -8995,7 +9061,7 @@
       <c r="C2" s="109" t="s">
         <v>170</v>
       </c>
-      <c r="D2"/>
+      <c r="D2" s="238"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="108"/>
@@ -9003,15 +9069,15 @@
       <c r="C3" s="122" t="s">
         <v>24</v>
       </c>
-      <c r="D3"/>
+      <c r="D3" s="238"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="108"/>
       <c r="B4" s="109"/>
-      <c r="C4" s="296" t="s">
+      <c r="C4" s="122" t="s">
         <v>130</v>
       </c>
-      <c r="D4"/>
+      <c r="D4" s="238"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="108"/>
@@ -9019,7 +9085,7 @@
       <c r="C5" s="122" t="s">
         <v>27</v>
       </c>
-      <c r="D5"/>
+      <c r="D5" s="238"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="108"/>
@@ -9027,7 +9093,7 @@
       <c r="C6" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="D6"/>
+      <c r="D6" s="238"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="108"/>
@@ -9035,7 +9101,7 @@
       <c r="C7" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="D7"/>
+      <c r="D7" s="238"/>
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="106" t="s">
@@ -9047,7 +9113,7 @@
       <c r="C8" s="107" t="s">
         <v>171</v>
       </c>
-      <c r="D8"/>
+      <c r="D8" s="238"/>
     </row>
     <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="108" t="s">
@@ -9059,7 +9125,7 @@
       <c r="C9" s="109" t="s">
         <v>172</v>
       </c>
-      <c r="D9"/>
+      <c r="D9" s="238"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="108"/>
@@ -9067,7 +9133,7 @@
       <c r="C10" s="122" t="s">
         <v>110</v>
       </c>
-      <c r="D10"/>
+      <c r="D10" s="238"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="108"/>
@@ -9075,7 +9141,7 @@
       <c r="C11" s="122" t="s">
         <v>111</v>
       </c>
-      <c r="D11"/>
+      <c r="D11" s="238"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="108"/>
@@ -9083,7 +9149,7 @@
       <c r="C12" s="122" t="s">
         <v>112</v>
       </c>
-      <c r="D12"/>
+      <c r="D12" s="238"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="108"/>
@@ -9091,7 +9157,7 @@
       <c r="C13" s="122" t="s">
         <v>113</v>
       </c>
-      <c r="D13"/>
+      <c r="D13" s="238"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="108"/>
@@ -9099,7 +9165,7 @@
       <c r="C14" s="203" t="s">
         <v>114</v>
       </c>
-      <c r="D14"/>
+      <c r="D14" s="238"/>
     </row>
     <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="106" t="s">
@@ -9111,7 +9177,7 @@
       <c r="C15" s="107" t="s">
         <v>173</v>
       </c>
-      <c r="D15"/>
+      <c r="D15" s="238"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="108" t="s">
@@ -9123,7 +9189,7 @@
       <c r="C16" s="109" t="s">
         <v>174</v>
       </c>
-      <c r="D16"/>
+      <c r="D16" s="238"/>
     </row>
     <row r="17" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="113" t="s">
@@ -9146,7 +9212,7 @@
       <c r="C18" s="161" t="s">
         <v>338</v>
       </c>
-      <c r="D18" s="276"/>
+      <c r="D18" s="237"/>
     </row>
     <row r="19" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="118" t="s">
@@ -9158,22 +9224,22 @@
       <c r="C19" s="156" t="s">
         <v>353</v>
       </c>
-      <c r="D19" s="276"/>
+      <c r="D19" s="237"/>
     </row>
     <row r="20" spans="1:4" s="289" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="293" t="s">
+      <c r="A20" s="300" t="s">
         <v>327</v>
       </c>
-      <c r="B20" s="293" t="s">
+      <c r="B20" s="300" t="s">
         <v>328</v>
       </c>
-      <c r="C20" s="293" t="s">
+      <c r="C20" s="300" t="s">
         <v>328</v>
       </c>
-      <c r="D20" s="276"/>
+      <c r="D20" s="237"/>
     </row>
     <row r="21" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="302" t="s">
+      <c r="A21" s="296" t="s">
         <v>326</v>
       </c>
       <c r="B21" s="116" t="s">
@@ -9182,46 +9248,51 @@
       <c r="C21" s="116" t="s">
         <v>176</v>
       </c>
-      <c r="D21"/>
+      <c r="D21" s="238"/>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="293" t="s">
+      <c r="A22" s="300" t="s">
         <v>329</v>
       </c>
-      <c r="B22" s="293" t="s">
+      <c r="B22" s="300" t="s">
         <v>330</v>
       </c>
-      <c r="C22" s="293" t="s">
+      <c r="C22" s="300" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="289"/>
-      <c r="C23" s="295" t="s">
+      <c r="A23" s="301"/>
+      <c r="B23" s="302"/>
+      <c r="C23" s="303" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="289"/>
-      <c r="C24" s="296" t="s">
+      <c r="A24" s="301"/>
+      <c r="B24" s="302"/>
+      <c r="C24" s="304" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="289"/>
-      <c r="C25" s="295" t="s">
+      <c r="A25" s="301"/>
+      <c r="B25" s="302"/>
+      <c r="C25" s="303" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="289"/>
-      <c r="C26" s="295" t="s">
+      <c r="A26" s="301"/>
+      <c r="B26" s="302"/>
+      <c r="C26" s="303" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="289"/>
-      <c r="C27" s="295" t="s">
+      <c r="A27" s="301"/>
+      <c r="B27" s="302"/>
+      <c r="C27" s="303" t="s">
         <v>29</v>
       </c>
     </row>
@@ -9234,8 +9305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K136"/>
   <sheetViews>
-    <sheetView topLeftCell="A154" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9857,7 +9928,7 @@
       <c r="C51" s="129" t="s">
         <v>190</v>
       </c>
-      <c r="D51"/>
+      <c r="D51" s="214"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="115"/>
@@ -10689,12 +10760,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC6C39E-D7F2-4BBD-963B-89B3F6A5164F}">
   <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="2" topLeftCell="G27" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E4" sqref="E4"/>
       <selection pane="topRight" activeCell="E4" sqref="E4"/>
       <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10719,11 +10790,11 @@
         <v>127</v>
       </c>
       <c r="D1" s="135"/>
-      <c r="E1" s="303" t="s">
+      <c r="E1" s="305" t="s">
         <v>247</v>
       </c>
-      <c r="F1" s="304"/>
-      <c r="G1" s="304"/>
+      <c r="F1" s="306"/>
+      <c r="G1" s="306"/>
     </row>
     <row r="2" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="109" t="s">
@@ -10945,7 +11016,7 @@
       <c r="A25" s="116" t="s">
         <v>188</v>
       </c>
-      <c r="B25" s="298" t="s">
+      <c r="B25" s="292" t="s">
         <v>350</v>
       </c>
       <c r="C25" s="153" t="s">
@@ -10981,7 +11052,7 @@
       <c r="A29" s="119" t="s">
         <v>188</v>
       </c>
-      <c r="B29" s="299" t="s">
+      <c r="B29" s="293" t="s">
         <v>352</v>
       </c>
       <c r="C29" s="156" t="s">
@@ -11066,7 +11137,7 @@
       <c r="D37" s="143"/>
     </row>
     <row r="38" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="297" t="s">
+      <c r="A38" s="118" t="s">
         <v>191</v>
       </c>
       <c r="B38" s="157"/>
@@ -11076,7 +11147,7 @@
       <c r="D38" s="150"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="297"/>
+      <c r="A39" s="118"/>
       <c r="B39" s="157" t="s">
         <v>251</v>
       </c>
@@ -11086,7 +11157,7 @@
       <c r="D39" s="143"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="297"/>
+      <c r="A40" s="118"/>
       <c r="B40" s="157" t="s">
         <v>251</v>
       </c>
@@ -11096,7 +11167,7 @@
       <c r="D40" s="143"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="297"/>
+      <c r="A41" s="118"/>
       <c r="B41" s="157" t="s">
         <v>251</v>
       </c>
@@ -11609,12 +11680,12 @@
       <c r="C2" s="109" t="s">
         <v>170</v>
       </c>
-      <c r="D2" s="305" t="s">
+      <c r="D2" s="307" t="s">
         <v>246</v>
       </c>
-      <c r="E2" s="306"/>
-      <c r="F2" s="306"/>
-      <c r="G2" s="306"/>
+      <c r="E2" s="308"/>
+      <c r="F2" s="308"/>
+      <c r="G2" s="308"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="106" t="s">
@@ -12101,7 +12172,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="297" t="s">
+      <c r="A65" s="291" t="s">
         <v>191</v>
       </c>
       <c r="B65" s="120"/>
@@ -12110,7 +12181,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="297"/>
+      <c r="A66" s="291"/>
       <c r="B66" s="120" t="s">
         <v>193</v>
       </c>
@@ -12119,7 +12190,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="297"/>
+      <c r="A67" s="291"/>
       <c r="B67" s="120" t="s">
         <v>194</v>
       </c>
@@ -12128,7 +12199,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="297"/>
+      <c r="A68" s="291"/>
       <c r="B68" s="120" t="s">
         <v>195</v>
       </c>
@@ -12137,7 +12208,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="297"/>
+      <c r="A69" s="291"/>
       <c r="B69" s="120" t="s">
         <v>196</v>
       </c>
@@ -12146,7 +12217,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="297"/>
+      <c r="A70" s="291"/>
       <c r="B70" s="120" t="s">
         <v>197</v>
       </c>
@@ -12155,7 +12226,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="297"/>
+      <c r="A71" s="291"/>
       <c r="B71" s="120" t="s">
         <v>198</v>
       </c>

</xml_diff>